<commit_message>
Pass in the secret key used for hashing as a dependency
</commit_message>
<xml_diff>
--- a/me/4.create-a-restful-api/6.authentication-using-json-web-tokens.xlsx
+++ b/me/4.create-a-restful-api/6.authentication-using-json-web-tokens.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\rest-api-php\me\4.create-a-restful-api\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A79FB9D-79FC-447D-8D97-BC313E2448A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4A81A7A-FAD3-49CC-B266-CAA597522D74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="introduction jwt" sheetId="1" r:id="rId1"/>
     <sheet name="encode a payload" sheetId="2" r:id="rId2"/>
     <sheet name="jwt containing claims in login " sheetId="3" r:id="rId3"/>
     <sheet name="decode payload from the JWT" sheetId="4" r:id="rId4"/>
+    <sheet name="use secret key as dependency" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="630" uniqueCount="229">
   <si>
     <t>An introduction to JSON web tokens (JWTs)</t>
   </si>
@@ -1788,6 +1789,73 @@
       <t>');</t>
     </r>
   </si>
+  <si>
+    <t>Pass in the secret key used for hashing as a dependency</t>
+  </si>
+  <si>
+    <t>bỏ đi phần test code</t>
+  </si>
+  <si>
+    <t>rest-api-php\4.create-a-restful-api\.env</t>
+  </si>
+  <si>
+    <t>DB_HOST="localhost"</t>
+  </si>
+  <si>
+    <t>DB_NAME="api_db"</t>
+  </si>
+  <si>
+    <t>DB_USER="root"</t>
+  </si>
+  <si>
+    <t>DB_PASS=""</t>
+  </si>
+  <si>
+    <t>SECRET_KEY="3979244226452948404D635166546A576E5A7234743777217A25432A462D4A61"</t>
+  </si>
+  <si>
+    <t>    private $key;</t>
+  </si>
+  <si>
+    <t>    public function __construct(string $key)</t>
+  </si>
+  <si>
+    <t>        $this-&gt;key = $key;</t>
+  </si>
+  <si>
+    <t>            $this-&gt;key,</t>
+  </si>
+  <si>
+    <r>
+      <t>$codec = new JWTCodec</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>($_ENV["SECRET_KEY"])</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <t>Giá trị secret trong class JWTCodec được dùng cả ở encode và decode, mình nên config nó trong file .env và truyền nó thông qua hàm khởi tạo __construct()</t>
+  </si>
+  <si>
+    <t>call api /login.php và thấy nó vẫn hoạt động bình thường và trả về chuỗi access token jwt</t>
+  </si>
 </sst>
 </file>
 
@@ -2038,7 +2106,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -2069,6 +2137,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5491,6 +5560,187 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>493743</xdr:colOff>
+      <xdr:row>98</xdr:row>
+      <xdr:rowOff>8965</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{987CDC92-F660-DE95-1A91-48B64FE21E79}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6324600" y="14201775"/>
+          <a:ext cx="12457143" cy="4476190"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>192</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>8175</xdr:colOff>
+      <xdr:row>198</xdr:row>
+      <xdr:rowOff>123671</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{467F620E-C2B8-F20C-A367-A41F50BEC495}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5667375" y="36614100"/>
+          <a:ext cx="10800000" cy="1228571"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>202</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>213</xdr:row>
+      <xdr:rowOff>83319</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{68F72C9D-8553-1A7B-BAE3-F3B2BFE768BB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="742950" y="38614350"/>
+          <a:ext cx="11306175" cy="2045469"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>218</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>379820</xdr:colOff>
+      <xdr:row>236</xdr:row>
+      <xdr:rowOff>56718</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{27CF5B0F-A7B4-1217-C574-40A4A3E64F81}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="695325" y="41557575"/>
+          <a:ext cx="9438095" cy="3457143"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -17419,8 +17669,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FA4BA49-D34B-4B6B-A6E4-9D7B28D9134C}">
   <dimension ref="A2:T340"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A334" workbookViewId="0">
-      <selection activeCell="H347" sqref="H347"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:L39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -22820,4 +23070,2854 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F919ACA-908A-4643-A7D8-BA9996B0FA16}">
+  <dimension ref="A2:T237"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A217" workbookViewId="0">
+      <selection activeCell="T221" sqref="T221"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="2" spans="1:10">
+      <c r="B2" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="B3" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="13"/>
+      <c r="B6" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="3"/>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="13"/>
+      <c r="B7" s="7"/>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="J7" s="6"/>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="13"/>
+      <c r="B8" s="7"/>
+      <c r="C8" t="s">
+        <v>18</v>
+      </c>
+      <c r="J8" s="6"/>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="13"/>
+      <c r="B9" s="7"/>
+      <c r="C9" t="s">
+        <v>19</v>
+      </c>
+      <c r="J9" s="6"/>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" s="13"/>
+      <c r="B10" s="7"/>
+      <c r="D10" t="s">
+        <v>20</v>
+      </c>
+      <c r="J10" s="6"/>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" s="13"/>
+      <c r="B11" s="7"/>
+      <c r="E11" t="s">
+        <v>21</v>
+      </c>
+      <c r="J11" s="6"/>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" s="13"/>
+      <c r="B12" s="7"/>
+      <c r="E12" t="s">
+        <v>22</v>
+      </c>
+      <c r="J12" s="6"/>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" s="13"/>
+      <c r="B13" s="7"/>
+      <c r="D13" t="s">
+        <v>23</v>
+      </c>
+      <c r="J13" s="6"/>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" s="13"/>
+      <c r="B14" s="7"/>
+      <c r="D14" t="s">
+        <v>24</v>
+      </c>
+      <c r="J14" s="6"/>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15" s="13"/>
+      <c r="B15" s="7"/>
+      <c r="D15" t="s">
+        <v>25</v>
+      </c>
+      <c r="J15" s="6"/>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16" s="13"/>
+      <c r="B16" s="7"/>
+      <c r="E16" t="s">
+        <v>26</v>
+      </c>
+      <c r="J16" s="6"/>
+    </row>
+    <row r="17" spans="1:12">
+      <c r="A17" s="13"/>
+      <c r="B17" s="7"/>
+      <c r="F17" t="s">
+        <v>27</v>
+      </c>
+      <c r="J17" s="6"/>
+    </row>
+    <row r="18" spans="1:12">
+      <c r="A18" s="13"/>
+      <c r="B18" s="7"/>
+      <c r="F18" t="s">
+        <v>28</v>
+      </c>
+      <c r="J18" s="6"/>
+    </row>
+    <row r="19" spans="1:12">
+      <c r="A19" s="13"/>
+      <c r="B19" s="7"/>
+      <c r="F19" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="J19" s="6"/>
+      <c r="K19" t="s">
+        <v>48</v>
+      </c>
+      <c r="L19" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
+      <c r="A20" s="13"/>
+      <c r="B20" s="7"/>
+      <c r="F20" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="J20" s="6"/>
+      <c r="K20" t="s">
+        <v>48</v>
+      </c>
+      <c r="L20" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
+      <c r="A21" s="13"/>
+      <c r="B21" s="7"/>
+      <c r="E21" t="s">
+        <v>30</v>
+      </c>
+      <c r="J21" s="6"/>
+    </row>
+    <row r="22" spans="1:12">
+      <c r="A22" s="13"/>
+      <c r="B22" s="7"/>
+      <c r="F22" t="s">
+        <v>31</v>
+      </c>
+      <c r="J22" s="6"/>
+    </row>
+    <row r="23" spans="1:12">
+      <c r="A23" s="13"/>
+      <c r="B23" s="7"/>
+      <c r="F23" t="s">
+        <v>32</v>
+      </c>
+      <c r="J23" s="6"/>
+    </row>
+    <row r="24" spans="1:12">
+      <c r="A24" s="13"/>
+      <c r="B24" s="7"/>
+      <c r="F24" t="s">
+        <v>33</v>
+      </c>
+      <c r="J24" s="6"/>
+    </row>
+    <row r="25" spans="1:12">
+      <c r="A25" s="13"/>
+      <c r="B25" s="7"/>
+      <c r="F25" t="s">
+        <v>34</v>
+      </c>
+      <c r="J25" s="6"/>
+    </row>
+    <row r="26" spans="1:12">
+      <c r="A26" s="13"/>
+      <c r="B26" s="7"/>
+      <c r="F26" t="s">
+        <v>35</v>
+      </c>
+      <c r="J26" s="6"/>
+    </row>
+    <row r="27" spans="1:12">
+      <c r="A27" s="13"/>
+      <c r="B27" s="7"/>
+      <c r="E27" t="s">
+        <v>36</v>
+      </c>
+      <c r="J27" s="6"/>
+    </row>
+    <row r="28" spans="1:12">
+      <c r="A28" s="13"/>
+      <c r="B28" s="7"/>
+      <c r="F28" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="J28" s="6"/>
+    </row>
+    <row r="29" spans="1:12">
+      <c r="A29" s="13"/>
+      <c r="B29" s="7"/>
+      <c r="F29" t="s">
+        <v>38</v>
+      </c>
+      <c r="J29" s="6"/>
+    </row>
+    <row r="30" spans="1:12">
+      <c r="A30" s="13"/>
+      <c r="B30" s="7"/>
+      <c r="F30" t="s">
+        <v>39</v>
+      </c>
+      <c r="J30" s="6"/>
+    </row>
+    <row r="31" spans="1:12">
+      <c r="A31" s="13"/>
+      <c r="B31" s="7"/>
+      <c r="F31" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="J31" s="6"/>
+      <c r="K31" t="s">
+        <v>48</v>
+      </c>
+      <c r="L31" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12">
+      <c r="A32" s="13"/>
+      <c r="B32" s="7"/>
+      <c r="F32" t="s">
+        <v>40</v>
+      </c>
+      <c r="J32" s="6"/>
+    </row>
+    <row r="33" spans="1:12">
+      <c r="A33" s="13"/>
+      <c r="B33" s="7"/>
+      <c r="F33" t="s">
+        <v>41</v>
+      </c>
+      <c r="J33" s="6"/>
+    </row>
+    <row r="34" spans="1:12">
+      <c r="A34" s="13"/>
+      <c r="B34" s="7"/>
+      <c r="F34" t="s">
+        <v>42</v>
+      </c>
+      <c r="J34" s="6"/>
+    </row>
+    <row r="35" spans="1:12">
+      <c r="A35" s="13"/>
+      <c r="B35" s="7"/>
+      <c r="E35" t="s">
+        <v>43</v>
+      </c>
+      <c r="J35" s="6"/>
+    </row>
+    <row r="36" spans="1:12">
+      <c r="A36" s="13"/>
+      <c r="B36" s="7"/>
+      <c r="E36" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="J36" s="6"/>
+      <c r="K36" t="s">
+        <v>48</v>
+      </c>
+      <c r="L36" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12">
+      <c r="A37" s="13"/>
+      <c r="B37" s="7"/>
+      <c r="E37" t="s">
+        <v>45</v>
+      </c>
+      <c r="J37" s="6"/>
+    </row>
+    <row r="38" spans="1:12">
+      <c r="A38" s="13"/>
+      <c r="B38" s="8"/>
+      <c r="C38" s="9"/>
+      <c r="D38" s="9"/>
+      <c r="E38" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="F38" s="9"/>
+      <c r="G38" s="9"/>
+      <c r="H38" s="9"/>
+      <c r="I38" s="9"/>
+      <c r="J38" s="10"/>
+    </row>
+    <row r="41" spans="1:12">
+      <c r="A41" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12">
+      <c r="B42" s="11" t="s">
+        <v>217</v>
+      </c>
+      <c r="C42" s="2"/>
+      <c r="D42" s="2"/>
+      <c r="E42" s="2"/>
+      <c r="F42" s="2"/>
+      <c r="G42" s="2"/>
+      <c r="H42" s="2"/>
+      <c r="I42" s="2"/>
+      <c r="J42" s="3"/>
+    </row>
+    <row r="43" spans="1:12">
+      <c r="B43" s="7" t="s">
+        <v>218</v>
+      </c>
+      <c r="C43" s="5"/>
+      <c r="D43" s="5"/>
+      <c r="E43" s="5"/>
+      <c r="F43" s="5"/>
+      <c r="G43" s="5"/>
+      <c r="H43" s="5"/>
+      <c r="I43" s="5"/>
+      <c r="J43" s="6"/>
+    </row>
+    <row r="44" spans="1:12">
+      <c r="B44" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="C44" s="5"/>
+      <c r="D44" s="5"/>
+      <c r="E44" s="5"/>
+      <c r="F44" s="5"/>
+      <c r="G44" s="5"/>
+      <c r="H44" s="5"/>
+      <c r="I44" s="5"/>
+      <c r="J44" s="6"/>
+    </row>
+    <row r="45" spans="1:12">
+      <c r="B45" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="C45" s="5"/>
+      <c r="D45" s="5"/>
+      <c r="E45" s="5"/>
+      <c r="F45" s="5"/>
+      <c r="G45" s="5"/>
+      <c r="H45" s="5"/>
+      <c r="I45" s="5"/>
+      <c r="J45" s="6"/>
+    </row>
+    <row r="46" spans="1:12">
+      <c r="B46" s="7"/>
+      <c r="C46" s="5"/>
+      <c r="D46" s="5"/>
+      <c r="E46" s="5"/>
+      <c r="F46" s="5"/>
+      <c r="G46" s="5"/>
+      <c r="H46" s="5"/>
+      <c r="I46" s="5"/>
+      <c r="J46" s="6"/>
+    </row>
+    <row r="47" spans="1:12">
+      <c r="B47" s="30" t="s">
+        <v>221</v>
+      </c>
+      <c r="C47" s="9"/>
+      <c r="D47" s="9"/>
+      <c r="E47" s="9"/>
+      <c r="F47" s="9"/>
+      <c r="G47" s="9"/>
+      <c r="H47" s="9"/>
+      <c r="I47" s="9"/>
+      <c r="J47" s="10"/>
+    </row>
+    <row r="50" spans="1:10">
+      <c r="A50" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10">
+      <c r="B51" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="C51" s="2"/>
+      <c r="D51" s="2"/>
+      <c r="E51" s="2"/>
+      <c r="F51" s="2"/>
+      <c r="G51" s="2"/>
+      <c r="H51" s="2"/>
+      <c r="I51" s="2"/>
+      <c r="J51" s="3"/>
+    </row>
+    <row r="52" spans="1:10">
+      <c r="B52" s="7"/>
+      <c r="C52" s="5"/>
+      <c r="D52" s="5"/>
+      <c r="E52" s="5"/>
+      <c r="F52" s="5"/>
+      <c r="G52" s="5"/>
+      <c r="H52" s="5"/>
+      <c r="I52" s="5"/>
+      <c r="J52" s="6"/>
+    </row>
+    <row r="53" spans="1:10">
+      <c r="B53" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C53" s="5"/>
+      <c r="D53" s="5"/>
+      <c r="E53" s="5"/>
+      <c r="F53" s="5"/>
+      <c r="G53" s="5"/>
+      <c r="H53" s="5"/>
+      <c r="I53" s="5"/>
+      <c r="J53" s="6"/>
+    </row>
+    <row r="54" spans="1:10">
+      <c r="B54" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C54" s="5"/>
+      <c r="D54" s="5"/>
+      <c r="E54" s="5"/>
+      <c r="F54" s="5"/>
+      <c r="G54" s="5"/>
+      <c r="H54" s="5"/>
+      <c r="I54" s="5"/>
+      <c r="J54" s="6"/>
+    </row>
+    <row r="55" spans="1:10">
+      <c r="B55" s="18" t="s">
+        <v>222</v>
+      </c>
+      <c r="C55" s="5"/>
+      <c r="D55" s="5"/>
+      <c r="E55" s="5"/>
+      <c r="F55" s="5"/>
+      <c r="G55" s="5"/>
+      <c r="H55" s="5"/>
+      <c r="I55" s="5"/>
+      <c r="J55" s="6"/>
+    </row>
+    <row r="56" spans="1:10">
+      <c r="B56" s="18"/>
+      <c r="C56" s="5"/>
+      <c r="D56" s="5"/>
+      <c r="E56" s="5"/>
+      <c r="F56" s="5"/>
+      <c r="G56" s="5"/>
+      <c r="H56" s="5"/>
+      <c r="I56" s="5"/>
+      <c r="J56" s="6"/>
+    </row>
+    <row r="57" spans="1:10">
+      <c r="B57" s="18" t="s">
+        <v>223</v>
+      </c>
+      <c r="C57" s="5"/>
+      <c r="D57" s="5"/>
+      <c r="E57" s="5"/>
+      <c r="F57" s="5"/>
+      <c r="G57" s="5"/>
+      <c r="H57" s="5"/>
+      <c r="I57" s="5"/>
+      <c r="J57" s="6"/>
+    </row>
+    <row r="58" spans="1:10">
+      <c r="B58" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="C58" s="5"/>
+      <c r="D58" s="5"/>
+      <c r="E58" s="5"/>
+      <c r="F58" s="5"/>
+      <c r="G58" s="5"/>
+      <c r="H58" s="5"/>
+      <c r="I58" s="5"/>
+      <c r="J58" s="6"/>
+    </row>
+    <row r="59" spans="1:10">
+      <c r="B59" s="18" t="s">
+        <v>224</v>
+      </c>
+      <c r="C59" s="5"/>
+      <c r="D59" s="5"/>
+      <c r="E59" s="5"/>
+      <c r="F59" s="5"/>
+      <c r="G59" s="5"/>
+      <c r="H59" s="5"/>
+      <c r="I59" s="5"/>
+      <c r="J59" s="6"/>
+    </row>
+    <row r="60" spans="1:10">
+      <c r="B60" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="C60" s="5"/>
+      <c r="D60" s="5"/>
+      <c r="E60" s="5"/>
+      <c r="F60" s="5"/>
+      <c r="G60" s="5"/>
+      <c r="H60" s="5"/>
+      <c r="I60" s="5"/>
+      <c r="J60" s="6"/>
+    </row>
+    <row r="61" spans="1:10">
+      <c r="B61" s="7"/>
+      <c r="C61" s="5"/>
+      <c r="D61" s="5"/>
+      <c r="E61" s="5"/>
+      <c r="F61" s="5"/>
+      <c r="G61" s="5"/>
+      <c r="H61" s="5"/>
+      <c r="I61" s="5"/>
+      <c r="J61" s="6"/>
+    </row>
+    <row r="62" spans="1:10">
+      <c r="B62" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C62" s="5"/>
+      <c r="D62" s="5"/>
+      <c r="E62" s="5"/>
+      <c r="F62" s="5"/>
+      <c r="G62" s="5"/>
+      <c r="H62" s="5"/>
+      <c r="I62" s="5"/>
+      <c r="J62" s="6"/>
+    </row>
+    <row r="63" spans="1:10">
+      <c r="B63" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C63" s="5"/>
+      <c r="D63" s="5"/>
+      <c r="E63" s="5"/>
+      <c r="F63" s="5"/>
+      <c r="G63" s="5"/>
+      <c r="H63" s="5"/>
+      <c r="I63" s="5"/>
+      <c r="J63" s="6"/>
+    </row>
+    <row r="64" spans="1:10">
+      <c r="B64" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C64" s="5"/>
+      <c r="D64" s="5"/>
+      <c r="E64" s="5"/>
+      <c r="F64" s="5"/>
+      <c r="G64" s="5"/>
+      <c r="H64" s="5"/>
+      <c r="I64" s="5"/>
+      <c r="J64" s="6"/>
+    </row>
+    <row r="65" spans="2:10">
+      <c r="B65" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C65" s="5"/>
+      <c r="D65" s="5"/>
+      <c r="E65" s="5"/>
+      <c r="F65" s="5"/>
+      <c r="G65" s="5"/>
+      <c r="H65" s="5"/>
+      <c r="I65" s="5"/>
+      <c r="J65" s="6"/>
+    </row>
+    <row r="66" spans="2:10">
+      <c r="B66" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C66" s="5"/>
+      <c r="D66" s="5"/>
+      <c r="E66" s="5"/>
+      <c r="F66" s="5"/>
+      <c r="G66" s="5"/>
+      <c r="H66" s="5"/>
+      <c r="I66" s="5"/>
+      <c r="J66" s="6"/>
+    </row>
+    <row r="67" spans="2:10">
+      <c r="B67" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C67" s="5"/>
+      <c r="D67" s="5"/>
+      <c r="E67" s="5"/>
+      <c r="F67" s="5"/>
+      <c r="G67" s="5"/>
+      <c r="H67" s="5"/>
+      <c r="I67" s="5"/>
+      <c r="J67" s="6"/>
+    </row>
+    <row r="68" spans="2:10">
+      <c r="B68" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C68" s="5"/>
+      <c r="D68" s="5"/>
+      <c r="E68" s="5"/>
+      <c r="F68" s="5"/>
+      <c r="G68" s="5"/>
+      <c r="H68" s="5"/>
+      <c r="I68" s="5"/>
+      <c r="J68" s="6"/>
+    </row>
+    <row r="69" spans="2:10">
+      <c r="B69" s="7"/>
+      <c r="C69" s="5"/>
+      <c r="D69" s="5"/>
+      <c r="E69" s="5"/>
+      <c r="F69" s="5"/>
+      <c r="G69" s="5"/>
+      <c r="H69" s="5"/>
+      <c r="I69" s="5"/>
+      <c r="J69" s="6"/>
+    </row>
+    <row r="70" spans="2:10">
+      <c r="B70" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C70" s="5"/>
+      <c r="D70" s="5"/>
+      <c r="E70" s="5"/>
+      <c r="F70" s="5"/>
+      <c r="G70" s="5"/>
+      <c r="H70" s="5"/>
+      <c r="I70" s="5"/>
+      <c r="J70" s="6"/>
+    </row>
+    <row r="71" spans="2:10">
+      <c r="B71" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C71" s="5"/>
+      <c r="D71" s="5"/>
+      <c r="E71" s="5"/>
+      <c r="F71" s="5"/>
+      <c r="G71" s="5"/>
+      <c r="H71" s="5"/>
+      <c r="I71" s="5"/>
+      <c r="J71" s="6"/>
+    </row>
+    <row r="72" spans="2:10">
+      <c r="B72" s="7"/>
+      <c r="C72" s="5"/>
+      <c r="D72" s="5"/>
+      <c r="E72" s="5"/>
+      <c r="F72" s="5"/>
+      <c r="G72" s="5"/>
+      <c r="H72" s="5"/>
+      <c r="I72" s="5"/>
+      <c r="J72" s="6"/>
+    </row>
+    <row r="73" spans="2:10">
+      <c r="B73" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C73" s="5"/>
+      <c r="D73" s="5"/>
+      <c r="E73" s="5"/>
+      <c r="F73" s="5"/>
+      <c r="G73" s="5"/>
+      <c r="H73" s="5"/>
+      <c r="I73" s="5"/>
+      <c r="J73" s="6"/>
+    </row>
+    <row r="74" spans="2:10">
+      <c r="B74" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C74" s="5"/>
+      <c r="D74" s="5"/>
+      <c r="E74" s="5"/>
+      <c r="F74" s="5"/>
+      <c r="G74" s="5"/>
+      <c r="H74" s="5"/>
+      <c r="I74" s="5"/>
+      <c r="J74" s="6"/>
+    </row>
+    <row r="75" spans="2:10">
+      <c r="B75" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C75" s="5"/>
+      <c r="D75" s="5"/>
+      <c r="E75" s="5"/>
+      <c r="F75" s="5"/>
+      <c r="G75" s="5"/>
+      <c r="H75" s="5"/>
+      <c r="I75" s="5"/>
+      <c r="J75" s="6"/>
+    </row>
+    <row r="76" spans="2:10">
+      <c r="B76" s="18" t="s">
+        <v>225</v>
+      </c>
+      <c r="C76" s="5"/>
+      <c r="D76" s="5"/>
+      <c r="E76" s="5"/>
+      <c r="F76" s="5"/>
+      <c r="G76" s="5"/>
+      <c r="H76" s="5"/>
+      <c r="I76" s="5"/>
+      <c r="J76" s="6"/>
+    </row>
+    <row r="77" spans="2:10">
+      <c r="B77" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="C77" s="5"/>
+      <c r="D77" s="5"/>
+      <c r="E77" s="5"/>
+      <c r="F77" s="5"/>
+      <c r="G77" s="5"/>
+      <c r="H77" s="5"/>
+      <c r="I77" s="5"/>
+      <c r="J77" s="6"/>
+    </row>
+    <row r="78" spans="2:10">
+      <c r="B78" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C78" s="5"/>
+      <c r="D78" s="5"/>
+      <c r="E78" s="5"/>
+      <c r="F78" s="5"/>
+      <c r="G78" s="5"/>
+      <c r="H78" s="5"/>
+      <c r="I78" s="5"/>
+      <c r="J78" s="6"/>
+    </row>
+    <row r="79" spans="2:10">
+      <c r="B79" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C79" s="5"/>
+      <c r="D79" s="5"/>
+      <c r="E79" s="5"/>
+      <c r="F79" s="5"/>
+      <c r="G79" s="5"/>
+      <c r="H79" s="5"/>
+      <c r="I79" s="5"/>
+      <c r="J79" s="6"/>
+    </row>
+    <row r="80" spans="2:10">
+      <c r="B80" s="7"/>
+      <c r="C80" s="5"/>
+      <c r="D80" s="5"/>
+      <c r="E80" s="5"/>
+      <c r="F80" s="5"/>
+      <c r="G80" s="5"/>
+      <c r="H80" s="5"/>
+      <c r="I80" s="5"/>
+      <c r="J80" s="6"/>
+    </row>
+    <row r="81" spans="2:10">
+      <c r="B81" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C81" s="5"/>
+      <c r="D81" s="5"/>
+      <c r="E81" s="5"/>
+      <c r="F81" s="5"/>
+      <c r="G81" s="5"/>
+      <c r="H81" s="5"/>
+      <c r="I81" s="5"/>
+      <c r="J81" s="6"/>
+    </row>
+    <row r="82" spans="2:10">
+      <c r="B82" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C82" s="5"/>
+      <c r="D82" s="5"/>
+      <c r="E82" s="5"/>
+      <c r="F82" s="5"/>
+      <c r="G82" s="5"/>
+      <c r="H82" s="5"/>
+      <c r="I82" s="5"/>
+      <c r="J82" s="6"/>
+    </row>
+    <row r="83" spans="2:10">
+      <c r="B83" s="7"/>
+      <c r="C83" s="5"/>
+      <c r="D83" s="5"/>
+      <c r="E83" s="5"/>
+      <c r="F83" s="5"/>
+      <c r="G83" s="5"/>
+      <c r="H83" s="5"/>
+      <c r="I83" s="5"/>
+      <c r="J83" s="6"/>
+    </row>
+    <row r="84" spans="2:10">
+      <c r="B84" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="C84" s="5"/>
+      <c r="D84" s="5"/>
+      <c r="E84" s="5"/>
+      <c r="F84" s="5"/>
+      <c r="G84" s="5"/>
+      <c r="H84" s="5"/>
+      <c r="I84" s="5"/>
+      <c r="J84" s="6"/>
+    </row>
+    <row r="85" spans="2:10">
+      <c r="B85" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C85" s="5"/>
+      <c r="D85" s="5"/>
+      <c r="E85" s="5"/>
+      <c r="F85" s="5"/>
+      <c r="G85" s="5"/>
+      <c r="H85" s="5"/>
+      <c r="I85" s="5"/>
+      <c r="J85" s="6"/>
+    </row>
+    <row r="86" spans="2:10">
+      <c r="B86" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="C86" s="5"/>
+      <c r="D86" s="5"/>
+      <c r="E86" s="5"/>
+      <c r="F86" s="5"/>
+      <c r="G86" s="5"/>
+      <c r="H86" s="5"/>
+      <c r="I86" s="5"/>
+      <c r="J86" s="6"/>
+    </row>
+    <row r="87" spans="2:10">
+      <c r="B87" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="C87" s="5"/>
+      <c r="D87" s="5"/>
+      <c r="E87" s="5"/>
+      <c r="F87" s="5"/>
+      <c r="G87" s="5"/>
+      <c r="H87" s="5"/>
+      <c r="I87" s="5"/>
+      <c r="J87" s="6"/>
+    </row>
+    <row r="88" spans="2:10">
+      <c r="B88" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="C88" s="5"/>
+      <c r="D88" s="5"/>
+      <c r="E88" s="5"/>
+      <c r="F88" s="5"/>
+      <c r="G88" s="5"/>
+      <c r="H88" s="5"/>
+      <c r="I88" s="5"/>
+      <c r="J88" s="6"/>
+    </row>
+    <row r="89" spans="2:10">
+      <c r="B89" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="C89" s="5"/>
+      <c r="D89" s="5"/>
+      <c r="E89" s="5"/>
+      <c r="F89" s="5"/>
+      <c r="G89" s="5"/>
+      <c r="H89" s="5"/>
+      <c r="I89" s="5"/>
+      <c r="J89" s="6"/>
+    </row>
+    <row r="90" spans="2:10">
+      <c r="B90" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="C90" s="5"/>
+      <c r="D90" s="5"/>
+      <c r="E90" s="5"/>
+      <c r="F90" s="5"/>
+      <c r="G90" s="5"/>
+      <c r="H90" s="5"/>
+      <c r="I90" s="5"/>
+      <c r="J90" s="6"/>
+    </row>
+    <row r="91" spans="2:10">
+      <c r="B91" s="7"/>
+      <c r="C91" s="5"/>
+      <c r="D91" s="5"/>
+      <c r="E91" s="5"/>
+      <c r="F91" s="5"/>
+      <c r="G91" s="5"/>
+      <c r="H91" s="5"/>
+      <c r="I91" s="5"/>
+      <c r="J91" s="6"/>
+    </row>
+    <row r="92" spans="2:10">
+      <c r="B92" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="C92" s="5"/>
+      <c r="D92" s="5"/>
+      <c r="E92" s="5"/>
+      <c r="F92" s="5"/>
+      <c r="G92" s="5"/>
+      <c r="H92" s="5"/>
+      <c r="I92" s="5"/>
+      <c r="J92" s="6"/>
+    </row>
+    <row r="93" spans="2:10">
+      <c r="B93" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="C93" s="5"/>
+      <c r="D93" s="5"/>
+      <c r="E93" s="5"/>
+      <c r="F93" s="5"/>
+      <c r="G93" s="5"/>
+      <c r="H93" s="5"/>
+      <c r="I93" s="5"/>
+      <c r="J93" s="6"/>
+    </row>
+    <row r="94" spans="2:10">
+      <c r="B94" s="7"/>
+      <c r="C94" s="5"/>
+      <c r="D94" s="5"/>
+      <c r="E94" s="5"/>
+      <c r="F94" s="5"/>
+      <c r="G94" s="5"/>
+      <c r="H94" s="5"/>
+      <c r="I94" s="5"/>
+      <c r="J94" s="6"/>
+    </row>
+    <row r="95" spans="2:10">
+      <c r="B95" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C95" s="5"/>
+      <c r="D95" s="5"/>
+      <c r="E95" s="5"/>
+      <c r="F95" s="5"/>
+      <c r="G95" s="5"/>
+      <c r="H95" s="5"/>
+      <c r="I95" s="5"/>
+      <c r="J95" s="6"/>
+    </row>
+    <row r="96" spans="2:10">
+      <c r="B96" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C96" s="5"/>
+      <c r="D96" s="5"/>
+      <c r="E96" s="5"/>
+      <c r="F96" s="5"/>
+      <c r="G96" s="5"/>
+      <c r="H96" s="5"/>
+      <c r="I96" s="5"/>
+      <c r="J96" s="6"/>
+    </row>
+    <row r="97" spans="2:10">
+      <c r="B97" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="C97" s="5"/>
+      <c r="D97" s="5"/>
+      <c r="E97" s="5"/>
+      <c r="F97" s="5"/>
+      <c r="G97" s="5"/>
+      <c r="H97" s="5"/>
+      <c r="I97" s="5"/>
+      <c r="J97" s="6"/>
+    </row>
+    <row r="98" spans="2:10">
+      <c r="B98" s="18" t="s">
+        <v>225</v>
+      </c>
+      <c r="C98" s="5"/>
+      <c r="D98" s="5"/>
+      <c r="E98" s="5"/>
+      <c r="F98" s="5"/>
+      <c r="G98" s="5"/>
+      <c r="H98" s="5"/>
+      <c r="I98" s="5"/>
+      <c r="J98" s="6"/>
+    </row>
+    <row r="99" spans="2:10">
+      <c r="B99" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="C99" s="5"/>
+      <c r="D99" s="5"/>
+      <c r="E99" s="5"/>
+      <c r="F99" s="5"/>
+      <c r="G99" s="5"/>
+      <c r="H99" s="5"/>
+      <c r="I99" s="5"/>
+      <c r="J99" s="6"/>
+    </row>
+    <row r="100" spans="2:10">
+      <c r="B100" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C100" s="5"/>
+      <c r="D100" s="5"/>
+      <c r="E100" s="5"/>
+      <c r="F100" s="5"/>
+      <c r="G100" s="5"/>
+      <c r="H100" s="5"/>
+      <c r="I100" s="5"/>
+      <c r="J100" s="6"/>
+    </row>
+    <row r="101" spans="2:10">
+      <c r="B101" s="7"/>
+      <c r="C101" s="5"/>
+      <c r="D101" s="5"/>
+      <c r="E101" s="5"/>
+      <c r="F101" s="5"/>
+      <c r="G101" s="5"/>
+      <c r="H101" s="5"/>
+      <c r="I101" s="5"/>
+      <c r="J101" s="6"/>
+    </row>
+    <row r="102" spans="2:10">
+      <c r="B102" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="C102" s="5"/>
+      <c r="D102" s="5"/>
+      <c r="E102" s="5"/>
+      <c r="F102" s="5"/>
+      <c r="G102" s="5"/>
+      <c r="H102" s="5"/>
+      <c r="I102" s="5"/>
+      <c r="J102" s="6"/>
+    </row>
+    <row r="103" spans="2:10">
+      <c r="B103" s="7"/>
+      <c r="C103" s="5"/>
+      <c r="D103" s="5"/>
+      <c r="E103" s="5"/>
+      <c r="F103" s="5"/>
+      <c r="G103" s="5"/>
+      <c r="H103" s="5"/>
+      <c r="I103" s="5"/>
+      <c r="J103" s="6"/>
+    </row>
+    <row r="104" spans="2:10">
+      <c r="B104" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="C104" s="5"/>
+      <c r="D104" s="5"/>
+      <c r="E104" s="5"/>
+      <c r="F104" s="5"/>
+      <c r="G104" s="5"/>
+      <c r="H104" s="5"/>
+      <c r="I104" s="5"/>
+      <c r="J104" s="6"/>
+    </row>
+    <row r="105" spans="2:10">
+      <c r="B105" s="7"/>
+      <c r="C105" s="5"/>
+      <c r="D105" s="5"/>
+      <c r="E105" s="5"/>
+      <c r="F105" s="5"/>
+      <c r="G105" s="5"/>
+      <c r="H105" s="5"/>
+      <c r="I105" s="5"/>
+      <c r="J105" s="6"/>
+    </row>
+    <row r="106" spans="2:10">
+      <c r="B106" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="C106" s="5"/>
+      <c r="D106" s="5"/>
+      <c r="E106" s="5"/>
+      <c r="F106" s="5"/>
+      <c r="G106" s="5"/>
+      <c r="H106" s="5"/>
+      <c r="I106" s="5"/>
+      <c r="J106" s="6"/>
+    </row>
+    <row r="107" spans="2:10">
+      <c r="B107" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="C107" s="5"/>
+      <c r="D107" s="5"/>
+      <c r="E107" s="5"/>
+      <c r="F107" s="5"/>
+      <c r="G107" s="5"/>
+      <c r="H107" s="5"/>
+      <c r="I107" s="5"/>
+      <c r="J107" s="6"/>
+    </row>
+    <row r="108" spans="2:10">
+      <c r="B108" s="7"/>
+      <c r="C108" s="5"/>
+      <c r="D108" s="5"/>
+      <c r="E108" s="5"/>
+      <c r="F108" s="5"/>
+      <c r="G108" s="5"/>
+      <c r="H108" s="5"/>
+      <c r="I108" s="5"/>
+      <c r="J108" s="6"/>
+    </row>
+    <row r="109" spans="2:10">
+      <c r="B109" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="C109" s="5"/>
+      <c r="D109" s="5"/>
+      <c r="E109" s="5"/>
+      <c r="F109" s="5"/>
+      <c r="G109" s="5"/>
+      <c r="H109" s="5"/>
+      <c r="I109" s="5"/>
+      <c r="J109" s="6"/>
+    </row>
+    <row r="110" spans="2:10">
+      <c r="B110" s="7"/>
+      <c r="C110" s="5"/>
+      <c r="D110" s="5"/>
+      <c r="E110" s="5"/>
+      <c r="F110" s="5"/>
+      <c r="G110" s="5"/>
+      <c r="H110" s="5"/>
+      <c r="I110" s="5"/>
+      <c r="J110" s="6"/>
+    </row>
+    <row r="111" spans="2:10">
+      <c r="B111" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="C111" s="5"/>
+      <c r="D111" s="5"/>
+      <c r="E111" s="5"/>
+      <c r="F111" s="5"/>
+      <c r="G111" s="5"/>
+      <c r="H111" s="5"/>
+      <c r="I111" s="5"/>
+      <c r="J111" s="6"/>
+    </row>
+    <row r="112" spans="2:10">
+      <c r="B112" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C112" s="5"/>
+      <c r="D112" s="5"/>
+      <c r="E112" s="5"/>
+      <c r="F112" s="5"/>
+      <c r="G112" s="5"/>
+      <c r="H112" s="5"/>
+      <c r="I112" s="5"/>
+      <c r="J112" s="6"/>
+    </row>
+    <row r="113" spans="2:10">
+      <c r="B113" s="7"/>
+      <c r="C113" s="5"/>
+      <c r="D113" s="5"/>
+      <c r="E113" s="5"/>
+      <c r="F113" s="5"/>
+      <c r="G113" s="5"/>
+      <c r="H113" s="5"/>
+      <c r="I113" s="5"/>
+      <c r="J113" s="6"/>
+    </row>
+    <row r="114" spans="2:10">
+      <c r="B114" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C114" s="5"/>
+      <c r="D114" s="5"/>
+      <c r="E114" s="5"/>
+      <c r="F114" s="5"/>
+      <c r="G114" s="5"/>
+      <c r="H114" s="5"/>
+      <c r="I114" s="5"/>
+      <c r="J114" s="6"/>
+    </row>
+    <row r="115" spans="2:10">
+      <c r="B115" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C115" s="5"/>
+      <c r="D115" s="5"/>
+      <c r="E115" s="5"/>
+      <c r="F115" s="5"/>
+      <c r="G115" s="5"/>
+      <c r="H115" s="5"/>
+      <c r="I115" s="5"/>
+      <c r="J115" s="6"/>
+    </row>
+    <row r="116" spans="2:10">
+      <c r="B116" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="C116" s="5"/>
+      <c r="D116" s="5"/>
+      <c r="E116" s="5"/>
+      <c r="F116" s="5"/>
+      <c r="G116" s="5"/>
+      <c r="H116" s="5"/>
+      <c r="I116" s="5"/>
+      <c r="J116" s="6"/>
+    </row>
+    <row r="117" spans="2:10">
+      <c r="B117" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C117" s="5"/>
+      <c r="D117" s="5"/>
+      <c r="E117" s="5"/>
+      <c r="F117" s="5"/>
+      <c r="G117" s="5"/>
+      <c r="H117" s="5"/>
+      <c r="I117" s="5"/>
+      <c r="J117" s="6"/>
+    </row>
+    <row r="118" spans="2:10">
+      <c r="B118" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="C118" s="5"/>
+      <c r="D118" s="5"/>
+      <c r="E118" s="5"/>
+      <c r="F118" s="5"/>
+      <c r="G118" s="5"/>
+      <c r="H118" s="5"/>
+      <c r="I118" s="5"/>
+      <c r="J118" s="6"/>
+    </row>
+    <row r="119" spans="2:10">
+      <c r="B119" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C119" s="5"/>
+      <c r="D119" s="5"/>
+      <c r="E119" s="5"/>
+      <c r="F119" s="5"/>
+      <c r="G119" s="5"/>
+      <c r="H119" s="5"/>
+      <c r="I119" s="5"/>
+      <c r="J119" s="6"/>
+    </row>
+    <row r="120" spans="2:10">
+      <c r="B120" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C120" s="5"/>
+      <c r="D120" s="5"/>
+      <c r="E120" s="5"/>
+      <c r="F120" s="5"/>
+      <c r="G120" s="5"/>
+      <c r="H120" s="5"/>
+      <c r="I120" s="5"/>
+      <c r="J120" s="6"/>
+    </row>
+    <row r="121" spans="2:10">
+      <c r="B121" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C121" s="5"/>
+      <c r="D121" s="5"/>
+      <c r="E121" s="5"/>
+      <c r="F121" s="5"/>
+      <c r="G121" s="5"/>
+      <c r="H121" s="5"/>
+      <c r="I121" s="5"/>
+      <c r="J121" s="6"/>
+    </row>
+    <row r="122" spans="2:10">
+      <c r="B122" s="7"/>
+      <c r="C122" s="5"/>
+      <c r="D122" s="5"/>
+      <c r="E122" s="5"/>
+      <c r="F122" s="5"/>
+      <c r="G122" s="5"/>
+      <c r="H122" s="5"/>
+      <c r="I122" s="5"/>
+      <c r="J122" s="6"/>
+    </row>
+    <row r="123" spans="2:10">
+      <c r="B123" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="C123" s="5"/>
+      <c r="D123" s="5"/>
+      <c r="E123" s="5"/>
+      <c r="F123" s="5"/>
+      <c r="G123" s="5"/>
+      <c r="H123" s="5"/>
+      <c r="I123" s="5"/>
+      <c r="J123" s="6"/>
+    </row>
+    <row r="124" spans="2:10">
+      <c r="B124" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C124" s="5"/>
+      <c r="D124" s="5"/>
+      <c r="E124" s="5"/>
+      <c r="F124" s="5"/>
+      <c r="G124" s="5"/>
+      <c r="H124" s="5"/>
+      <c r="I124" s="5"/>
+      <c r="J124" s="6"/>
+    </row>
+    <row r="125" spans="2:10">
+      <c r="B125" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="C125" s="5"/>
+      <c r="D125" s="5"/>
+      <c r="E125" s="5"/>
+      <c r="F125" s="5"/>
+      <c r="G125" s="5"/>
+      <c r="H125" s="5"/>
+      <c r="I125" s="5"/>
+      <c r="J125" s="6"/>
+    </row>
+    <row r="126" spans="2:10">
+      <c r="B126" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="C126" s="5"/>
+      <c r="D126" s="5"/>
+      <c r="E126" s="5"/>
+      <c r="F126" s="5"/>
+      <c r="G126" s="5"/>
+      <c r="H126" s="5"/>
+      <c r="I126" s="5"/>
+      <c r="J126" s="6"/>
+    </row>
+    <row r="127" spans="2:10">
+      <c r="B127" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="C127" s="5"/>
+      <c r="D127" s="5"/>
+      <c r="E127" s="5"/>
+      <c r="F127" s="5"/>
+      <c r="G127" s="5"/>
+      <c r="H127" s="5"/>
+      <c r="I127" s="5"/>
+      <c r="J127" s="6"/>
+    </row>
+    <row r="128" spans="2:10">
+      <c r="B128" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="C128" s="5"/>
+      <c r="D128" s="5"/>
+      <c r="E128" s="5"/>
+      <c r="F128" s="5"/>
+      <c r="G128" s="5"/>
+      <c r="H128" s="5"/>
+      <c r="I128" s="5"/>
+      <c r="J128" s="6"/>
+    </row>
+    <row r="129" spans="1:10">
+      <c r="B129" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="C129" s="5"/>
+      <c r="D129" s="5"/>
+      <c r="E129" s="5"/>
+      <c r="F129" s="5"/>
+      <c r="G129" s="5"/>
+      <c r="H129" s="5"/>
+      <c r="I129" s="5"/>
+      <c r="J129" s="6"/>
+    </row>
+    <row r="130" spans="1:10">
+      <c r="B130" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="C130" s="5"/>
+      <c r="D130" s="5"/>
+      <c r="E130" s="5"/>
+      <c r="F130" s="5"/>
+      <c r="G130" s="5"/>
+      <c r="H130" s="5"/>
+      <c r="I130" s="5"/>
+      <c r="J130" s="6"/>
+    </row>
+    <row r="131" spans="1:10">
+      <c r="B131" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C131" s="5"/>
+      <c r="D131" s="5"/>
+      <c r="E131" s="5"/>
+      <c r="F131" s="5"/>
+      <c r="G131" s="5"/>
+      <c r="H131" s="5"/>
+      <c r="I131" s="5"/>
+      <c r="J131" s="6"/>
+    </row>
+    <row r="132" spans="1:10">
+      <c r="B132" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C132" s="5"/>
+      <c r="D132" s="5"/>
+      <c r="E132" s="5"/>
+      <c r="F132" s="5"/>
+      <c r="G132" s="5"/>
+      <c r="H132" s="5"/>
+      <c r="I132" s="5"/>
+      <c r="J132" s="6"/>
+    </row>
+    <row r="133" spans="1:10">
+      <c r="B133" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="C133" s="9"/>
+      <c r="D133" s="9"/>
+      <c r="E133" s="9"/>
+      <c r="F133" s="9"/>
+      <c r="G133" s="9"/>
+      <c r="H133" s="9"/>
+      <c r="I133" s="9"/>
+      <c r="J133" s="10"/>
+    </row>
+    <row r="136" spans="1:10">
+      <c r="A136" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="137" spans="1:10">
+      <c r="B137" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="C137" s="2"/>
+      <c r="D137" s="2"/>
+      <c r="E137" s="2"/>
+      <c r="F137" s="2"/>
+      <c r="G137" s="2"/>
+      <c r="H137" s="2"/>
+      <c r="I137" s="3"/>
+    </row>
+    <row r="138" spans="1:10">
+      <c r="B138" s="7"/>
+      <c r="C138" s="5"/>
+      <c r="D138" s="5"/>
+      <c r="E138" s="5"/>
+      <c r="F138" s="5"/>
+      <c r="G138" s="5"/>
+      <c r="H138" s="5"/>
+      <c r="I138" s="6"/>
+    </row>
+    <row r="139" spans="1:10">
+      <c r="B139" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="C139" s="5"/>
+      <c r="D139" s="5"/>
+      <c r="E139" s="5"/>
+      <c r="F139" s="5"/>
+      <c r="G139" s="5"/>
+      <c r="H139" s="5"/>
+      <c r="I139" s="6"/>
+    </row>
+    <row r="140" spans="1:10">
+      <c r="B140" s="7"/>
+      <c r="C140" s="5"/>
+      <c r="D140" s="5"/>
+      <c r="E140" s="5"/>
+      <c r="F140" s="5"/>
+      <c r="G140" s="5"/>
+      <c r="H140" s="5"/>
+      <c r="I140" s="6"/>
+    </row>
+    <row r="141" spans="1:10">
+      <c r="B141" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="C141" s="5"/>
+      <c r="D141" s="5"/>
+      <c r="E141" s="5"/>
+      <c r="F141" s="5"/>
+      <c r="G141" s="5"/>
+      <c r="H141" s="5"/>
+      <c r="I141" s="6"/>
+    </row>
+    <row r="142" spans="1:10">
+      <c r="B142" s="7"/>
+      <c r="C142" s="5"/>
+      <c r="D142" s="5"/>
+      <c r="E142" s="5"/>
+      <c r="F142" s="5"/>
+      <c r="G142" s="5"/>
+      <c r="H142" s="5"/>
+      <c r="I142" s="6"/>
+    </row>
+    <row r="143" spans="1:10">
+      <c r="B143" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="C143" s="5"/>
+      <c r="D143" s="5"/>
+      <c r="E143" s="5"/>
+      <c r="F143" s="5"/>
+      <c r="G143" s="5"/>
+      <c r="H143" s="5"/>
+      <c r="I143" s="6"/>
+    </row>
+    <row r="144" spans="1:10">
+      <c r="B144" s="7"/>
+      <c r="C144" s="5"/>
+      <c r="D144" s="5"/>
+      <c r="E144" s="5"/>
+      <c r="F144" s="5"/>
+      <c r="G144" s="5"/>
+      <c r="H144" s="5"/>
+      <c r="I144" s="6"/>
+    </row>
+    <row r="145" spans="2:9">
+      <c r="B145" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="C145" s="5"/>
+      <c r="D145" s="5"/>
+      <c r="E145" s="5"/>
+      <c r="F145" s="5"/>
+      <c r="G145" s="5"/>
+      <c r="H145" s="5"/>
+      <c r="I145" s="6"/>
+    </row>
+    <row r="146" spans="2:9">
+      <c r="B146" s="7"/>
+      <c r="C146" s="5"/>
+      <c r="D146" s="5"/>
+      <c r="E146" s="5"/>
+      <c r="F146" s="5"/>
+      <c r="G146" s="5"/>
+      <c r="H146" s="5"/>
+      <c r="I146" s="6"/>
+    </row>
+    <row r="147" spans="2:9">
+      <c r="B147" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="C147" s="5"/>
+      <c r="D147" s="5"/>
+      <c r="E147" s="5"/>
+      <c r="F147" s="5"/>
+      <c r="G147" s="5"/>
+      <c r="H147" s="5"/>
+      <c r="I147" s="6"/>
+    </row>
+    <row r="148" spans="2:9">
+      <c r="B148" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="C148" s="5"/>
+      <c r="D148" s="5"/>
+      <c r="E148" s="5"/>
+      <c r="F148" s="5"/>
+      <c r="G148" s="5"/>
+      <c r="H148" s="5"/>
+      <c r="I148" s="6"/>
+    </row>
+    <row r="149" spans="2:9">
+      <c r="B149" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="C149" s="5"/>
+      <c r="D149" s="5"/>
+      <c r="E149" s="5"/>
+      <c r="F149" s="5"/>
+      <c r="G149" s="5"/>
+      <c r="H149" s="5"/>
+      <c r="I149" s="6"/>
+    </row>
+    <row r="150" spans="2:9">
+      <c r="B150" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="C150" s="5"/>
+      <c r="D150" s="5"/>
+      <c r="E150" s="5"/>
+      <c r="F150" s="5"/>
+      <c r="G150" s="5"/>
+      <c r="H150" s="5"/>
+      <c r="I150" s="6"/>
+    </row>
+    <row r="151" spans="2:9">
+      <c r="B151" s="7"/>
+      <c r="C151" s="5"/>
+      <c r="D151" s="5"/>
+      <c r="E151" s="5"/>
+      <c r="F151" s="5"/>
+      <c r="G151" s="5"/>
+      <c r="H151" s="5"/>
+      <c r="I151" s="6"/>
+    </row>
+    <row r="152" spans="2:9">
+      <c r="B152" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="C152" s="5"/>
+      <c r="D152" s="5"/>
+      <c r="E152" s="5"/>
+      <c r="F152" s="5"/>
+      <c r="G152" s="5"/>
+      <c r="H152" s="5"/>
+      <c r="I152" s="6"/>
+    </row>
+    <row r="153" spans="2:9">
+      <c r="B153" s="7"/>
+      <c r="C153" s="5"/>
+      <c r="D153" s="5"/>
+      <c r="E153" s="5"/>
+      <c r="F153" s="5"/>
+      <c r="G153" s="5"/>
+      <c r="H153" s="5"/>
+      <c r="I153" s="6"/>
+    </row>
+    <row r="154" spans="2:9">
+      <c r="B154" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="C154" s="5"/>
+      <c r="D154" s="5"/>
+      <c r="E154" s="5"/>
+      <c r="F154" s="5"/>
+      <c r="G154" s="5"/>
+      <c r="H154" s="5"/>
+      <c r="I154" s="6"/>
+    </row>
+    <row r="155" spans="2:9">
+      <c r="B155" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="C155" s="5"/>
+      <c r="D155" s="5"/>
+      <c r="E155" s="5"/>
+      <c r="F155" s="5"/>
+      <c r="G155" s="5"/>
+      <c r="H155" s="5"/>
+      <c r="I155" s="6"/>
+    </row>
+    <row r="156" spans="2:9">
+      <c r="B156" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="C156" s="5"/>
+      <c r="D156" s="5"/>
+      <c r="E156" s="5"/>
+      <c r="F156" s="5"/>
+      <c r="G156" s="5"/>
+      <c r="H156" s="5"/>
+      <c r="I156" s="6"/>
+    </row>
+    <row r="157" spans="2:9">
+      <c r="B157" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="C157" s="5"/>
+      <c r="D157" s="5"/>
+      <c r="E157" s="5"/>
+      <c r="F157" s="5"/>
+      <c r="G157" s="5"/>
+      <c r="H157" s="5"/>
+      <c r="I157" s="6"/>
+    </row>
+    <row r="158" spans="2:9">
+      <c r="B158" s="7"/>
+      <c r="C158" s="5"/>
+      <c r="D158" s="5"/>
+      <c r="E158" s="5"/>
+      <c r="F158" s="5"/>
+      <c r="G158" s="5"/>
+      <c r="H158" s="5"/>
+      <c r="I158" s="6"/>
+    </row>
+    <row r="159" spans="2:9">
+      <c r="B159" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="C159" s="5"/>
+      <c r="D159" s="5"/>
+      <c r="E159" s="5"/>
+      <c r="F159" s="5"/>
+      <c r="G159" s="5"/>
+      <c r="H159" s="5"/>
+      <c r="I159" s="6"/>
+    </row>
+    <row r="160" spans="2:9">
+      <c r="B160" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="C160" s="5"/>
+      <c r="D160" s="5"/>
+      <c r="E160" s="5"/>
+      <c r="F160" s="5"/>
+      <c r="G160" s="5"/>
+      <c r="H160" s="5"/>
+      <c r="I160" s="6"/>
+    </row>
+    <row r="161" spans="2:9">
+      <c r="B161" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="C161" s="5"/>
+      <c r="D161" s="5"/>
+      <c r="E161" s="5"/>
+      <c r="F161" s="5"/>
+      <c r="G161" s="5"/>
+      <c r="H161" s="5"/>
+      <c r="I161" s="6"/>
+    </row>
+    <row r="162" spans="2:9">
+      <c r="B162" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="C162" s="5"/>
+      <c r="D162" s="5"/>
+      <c r="E162" s="5"/>
+      <c r="F162" s="5"/>
+      <c r="G162" s="5"/>
+      <c r="H162" s="5"/>
+      <c r="I162" s="6"/>
+    </row>
+    <row r="163" spans="2:9">
+      <c r="B163" s="7"/>
+      <c r="C163" s="5"/>
+      <c r="D163" s="5"/>
+      <c r="E163" s="5"/>
+      <c r="F163" s="5"/>
+      <c r="G163" s="5"/>
+      <c r="H163" s="5"/>
+      <c r="I163" s="6"/>
+    </row>
+    <row r="164" spans="2:9">
+      <c r="B164" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="C164" s="5"/>
+      <c r="D164" s="5"/>
+      <c r="E164" s="5"/>
+      <c r="F164" s="5"/>
+      <c r="G164" s="5"/>
+      <c r="H164" s="5"/>
+      <c r="I164" s="6"/>
+    </row>
+    <row r="165" spans="2:9">
+      <c r="B165" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="C165" s="5"/>
+      <c r="D165" s="5"/>
+      <c r="E165" s="5"/>
+      <c r="F165" s="5"/>
+      <c r="G165" s="5"/>
+      <c r="H165" s="5"/>
+      <c r="I165" s="6"/>
+    </row>
+    <row r="166" spans="2:9">
+      <c r="B166" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="C166" s="5"/>
+      <c r="D166" s="5"/>
+      <c r="E166" s="5"/>
+      <c r="F166" s="5"/>
+      <c r="G166" s="5"/>
+      <c r="H166" s="5"/>
+      <c r="I166" s="6"/>
+    </row>
+    <row r="167" spans="2:9">
+      <c r="B167" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="C167" s="5"/>
+      <c r="D167" s="5"/>
+      <c r="E167" s="5"/>
+      <c r="F167" s="5"/>
+      <c r="G167" s="5"/>
+      <c r="H167" s="5"/>
+      <c r="I167" s="6"/>
+    </row>
+    <row r="168" spans="2:9">
+      <c r="B168" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="C168" s="5"/>
+      <c r="D168" s="5"/>
+      <c r="E168" s="5"/>
+      <c r="F168" s="5"/>
+      <c r="G168" s="5"/>
+      <c r="H168" s="5"/>
+      <c r="I168" s="6"/>
+    </row>
+    <row r="169" spans="2:9">
+      <c r="B169" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="C169" s="5"/>
+      <c r="D169" s="5"/>
+      <c r="E169" s="5"/>
+      <c r="F169" s="5"/>
+      <c r="G169" s="5"/>
+      <c r="H169" s="5"/>
+      <c r="I169" s="6"/>
+    </row>
+    <row r="170" spans="2:9">
+      <c r="B170" s="7"/>
+      <c r="C170" s="5"/>
+      <c r="D170" s="5"/>
+      <c r="E170" s="5"/>
+      <c r="F170" s="5"/>
+      <c r="G170" s="5"/>
+      <c r="H170" s="5"/>
+      <c r="I170" s="6"/>
+    </row>
+    <row r="171" spans="2:9">
+      <c r="B171" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="C171" s="5"/>
+      <c r="D171" s="5"/>
+      <c r="E171" s="5"/>
+      <c r="F171" s="5"/>
+      <c r="G171" s="5"/>
+      <c r="H171" s="5"/>
+      <c r="I171" s="6"/>
+    </row>
+    <row r="172" spans="2:9">
+      <c r="B172" s="7"/>
+      <c r="C172" s="5"/>
+      <c r="D172" s="5"/>
+      <c r="E172" s="5"/>
+      <c r="F172" s="5"/>
+      <c r="G172" s="5"/>
+      <c r="H172" s="5"/>
+      <c r="I172" s="6"/>
+    </row>
+    <row r="173" spans="2:9">
+      <c r="B173" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="C173" s="5"/>
+      <c r="D173" s="5"/>
+      <c r="E173" s="5"/>
+      <c r="F173" s="5"/>
+      <c r="G173" s="5"/>
+      <c r="H173" s="5"/>
+      <c r="I173" s="6"/>
+    </row>
+    <row r="174" spans="2:9">
+      <c r="B174" s="7"/>
+      <c r="C174" s="5"/>
+      <c r="D174" s="5"/>
+      <c r="E174" s="5"/>
+      <c r="F174" s="5"/>
+      <c r="G174" s="5"/>
+      <c r="H174" s="5"/>
+      <c r="I174" s="6"/>
+    </row>
+    <row r="175" spans="2:9">
+      <c r="B175" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="C175" s="5"/>
+      <c r="D175" s="5"/>
+      <c r="E175" s="5"/>
+      <c r="F175" s="5"/>
+      <c r="G175" s="5"/>
+      <c r="H175" s="5"/>
+      <c r="I175" s="6"/>
+    </row>
+    <row r="176" spans="2:9">
+      <c r="B176" s="7"/>
+      <c r="C176" s="5"/>
+      <c r="D176" s="5"/>
+      <c r="E176" s="5"/>
+      <c r="F176" s="5"/>
+      <c r="G176" s="5"/>
+      <c r="H176" s="5"/>
+      <c r="I176" s="6"/>
+    </row>
+    <row r="177" spans="2:9">
+      <c r="B177" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="C177" s="5"/>
+      <c r="D177" s="5"/>
+      <c r="E177" s="5"/>
+      <c r="F177" s="5"/>
+      <c r="G177" s="5"/>
+      <c r="H177" s="5"/>
+      <c r="I177" s="6"/>
+    </row>
+    <row r="178" spans="2:9">
+      <c r="B178" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="C178" s="5"/>
+      <c r="D178" s="5"/>
+      <c r="E178" s="5"/>
+      <c r="F178" s="5"/>
+      <c r="G178" s="5"/>
+      <c r="H178" s="5"/>
+      <c r="I178" s="6"/>
+    </row>
+    <row r="179" spans="2:9">
+      <c r="B179" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="C179" s="5"/>
+      <c r="D179" s="5"/>
+      <c r="E179" s="5"/>
+      <c r="F179" s="5"/>
+      <c r="G179" s="5"/>
+      <c r="H179" s="5"/>
+      <c r="I179" s="6"/>
+    </row>
+    <row r="180" spans="2:9">
+      <c r="B180" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="C180" s="5"/>
+      <c r="D180" s="5"/>
+      <c r="E180" s="5"/>
+      <c r="F180" s="5"/>
+      <c r="G180" s="5"/>
+      <c r="H180" s="5"/>
+      <c r="I180" s="6"/>
+    </row>
+    <row r="181" spans="2:9">
+      <c r="B181" s="7"/>
+      <c r="C181" s="5"/>
+      <c r="D181" s="5"/>
+      <c r="E181" s="5"/>
+      <c r="F181" s="5"/>
+      <c r="G181" s="5"/>
+      <c r="H181" s="5"/>
+      <c r="I181" s="6"/>
+    </row>
+    <row r="182" spans="2:9">
+      <c r="B182" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="C182" s="5"/>
+      <c r="D182" s="5"/>
+      <c r="E182" s="5"/>
+      <c r="F182" s="5"/>
+      <c r="G182" s="5"/>
+      <c r="H182" s="5"/>
+      <c r="I182" s="6"/>
+    </row>
+    <row r="183" spans="2:9">
+      <c r="B183" s="7"/>
+      <c r="C183" s="5"/>
+      <c r="D183" s="5"/>
+      <c r="E183" s="5"/>
+      <c r="F183" s="5"/>
+      <c r="G183" s="5"/>
+      <c r="H183" s="5"/>
+      <c r="I183" s="6"/>
+    </row>
+    <row r="184" spans="2:9">
+      <c r="B184" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="C184" s="5"/>
+      <c r="D184" s="5"/>
+      <c r="E184" s="5"/>
+      <c r="F184" s="5"/>
+      <c r="G184" s="5"/>
+      <c r="H184" s="5"/>
+      <c r="I184" s="6"/>
+    </row>
+    <row r="185" spans="2:9">
+      <c r="B185" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="C185" s="5"/>
+      <c r="D185" s="5"/>
+      <c r="E185" s="5"/>
+      <c r="F185" s="5"/>
+      <c r="G185" s="5"/>
+      <c r="H185" s="5"/>
+      <c r="I185" s="6"/>
+    </row>
+    <row r="186" spans="2:9">
+      <c r="B186" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="C186" s="5"/>
+      <c r="D186" s="5"/>
+      <c r="E186" s="5"/>
+      <c r="F186" s="5"/>
+      <c r="G186" s="5"/>
+      <c r="H186" s="5"/>
+      <c r="I186" s="6"/>
+    </row>
+    <row r="187" spans="2:9">
+      <c r="B187" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="C187" s="5"/>
+      <c r="D187" s="5"/>
+      <c r="E187" s="5"/>
+      <c r="F187" s="5"/>
+      <c r="G187" s="5"/>
+      <c r="H187" s="5"/>
+      <c r="I187" s="6"/>
+    </row>
+    <row r="188" spans="2:9">
+      <c r="B188" s="7"/>
+      <c r="C188" s="5"/>
+      <c r="D188" s="5"/>
+      <c r="E188" s="5"/>
+      <c r="F188" s="5"/>
+      <c r="G188" s="5"/>
+      <c r="H188" s="5"/>
+      <c r="I188" s="6"/>
+    </row>
+    <row r="189" spans="2:9">
+      <c r="B189" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="C189" s="5"/>
+      <c r="D189" s="5"/>
+      <c r="E189" s="5"/>
+      <c r="F189" s="5"/>
+      <c r="G189" s="5"/>
+      <c r="H189" s="5"/>
+      <c r="I189" s="6"/>
+    </row>
+    <row r="190" spans="2:9">
+      <c r="B190" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="C190" s="5"/>
+      <c r="D190" s="5"/>
+      <c r="E190" s="5"/>
+      <c r="F190" s="5"/>
+      <c r="G190" s="5"/>
+      <c r="H190" s="5"/>
+      <c r="I190" s="6"/>
+    </row>
+    <row r="191" spans="2:9">
+      <c r="B191" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="C191" s="5"/>
+      <c r="D191" s="5"/>
+      <c r="E191" s="5"/>
+      <c r="F191" s="5"/>
+      <c r="G191" s="5"/>
+      <c r="H191" s="5"/>
+      <c r="I191" s="6"/>
+    </row>
+    <row r="192" spans="2:9">
+      <c r="B192" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="C192" s="5"/>
+      <c r="D192" s="5"/>
+      <c r="E192" s="5"/>
+      <c r="F192" s="5"/>
+      <c r="G192" s="5"/>
+      <c r="H192" s="5"/>
+      <c r="I192" s="6"/>
+    </row>
+    <row r="193" spans="1:20">
+      <c r="B193" s="7"/>
+      <c r="C193" s="5"/>
+      <c r="D193" s="5"/>
+      <c r="E193" s="5"/>
+      <c r="F193" s="5"/>
+      <c r="G193" s="5"/>
+      <c r="H193" s="5"/>
+      <c r="I193" s="6"/>
+    </row>
+    <row r="194" spans="1:20">
+      <c r="B194" s="7" t="s">
+        <v>226</v>
+      </c>
+      <c r="C194" s="5"/>
+      <c r="D194" s="5"/>
+      <c r="E194" s="5"/>
+      <c r="F194" s="5"/>
+      <c r="G194" s="5"/>
+      <c r="H194" s="5"/>
+      <c r="I194" s="6"/>
+    </row>
+    <row r="195" spans="1:20">
+      <c r="B195" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="C195" s="5"/>
+      <c r="D195" s="5"/>
+      <c r="E195" s="5"/>
+      <c r="F195" s="5"/>
+      <c r="G195" s="5"/>
+      <c r="H195" s="5"/>
+      <c r="I195" s="6"/>
+    </row>
+    <row r="196" spans="1:20">
+      <c r="B196" s="7"/>
+      <c r="C196" s="5"/>
+      <c r="D196" s="5"/>
+      <c r="E196" s="5"/>
+      <c r="F196" s="5"/>
+      <c r="G196" s="5"/>
+      <c r="H196" s="5"/>
+      <c r="I196" s="6"/>
+    </row>
+    <row r="197" spans="1:20">
+      <c r="B197" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="C197" s="5"/>
+      <c r="D197" s="5"/>
+      <c r="E197" s="5"/>
+      <c r="F197" s="5"/>
+      <c r="G197" s="5"/>
+      <c r="H197" s="5"/>
+      <c r="I197" s="6"/>
+    </row>
+    <row r="198" spans="1:20">
+      <c r="B198" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="C198" s="5"/>
+      <c r="D198" s="5"/>
+      <c r="E198" s="5"/>
+      <c r="F198" s="5"/>
+      <c r="G198" s="5"/>
+      <c r="H198" s="5"/>
+      <c r="I198" s="6"/>
+    </row>
+    <row r="199" spans="1:20">
+      <c r="B199" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="C199" s="9"/>
+      <c r="D199" s="9"/>
+      <c r="E199" s="9"/>
+      <c r="F199" s="9"/>
+      <c r="G199" s="9"/>
+      <c r="H199" s="9"/>
+      <c r="I199" s="10"/>
+    </row>
+    <row r="202" spans="1:20">
+      <c r="A202" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="203" spans="1:20">
+      <c r="B203" s="11"/>
+      <c r="C203" s="2"/>
+      <c r="D203" s="2"/>
+      <c r="E203" s="2"/>
+      <c r="F203" s="2"/>
+      <c r="G203" s="2"/>
+      <c r="H203" s="2"/>
+      <c r="I203" s="2"/>
+      <c r="J203" s="2"/>
+      <c r="K203" s="2"/>
+      <c r="L203" s="2"/>
+      <c r="M203" s="2"/>
+      <c r="N203" s="2"/>
+      <c r="O203" s="2"/>
+      <c r="P203" s="2"/>
+      <c r="Q203" s="2"/>
+      <c r="R203" s="2"/>
+      <c r="S203" s="2"/>
+      <c r="T203" s="3"/>
+    </row>
+    <row r="204" spans="1:20">
+      <c r="B204" s="7"/>
+      <c r="C204" s="5"/>
+      <c r="D204" s="5"/>
+      <c r="E204" s="5"/>
+      <c r="F204" s="5"/>
+      <c r="G204" s="5"/>
+      <c r="H204" s="5"/>
+      <c r="I204" s="5"/>
+      <c r="J204" s="5"/>
+      <c r="K204" s="5"/>
+      <c r="L204" s="5"/>
+      <c r="M204" s="5"/>
+      <c r="N204" s="5"/>
+      <c r="O204" s="5"/>
+      <c r="P204" s="5"/>
+      <c r="Q204" s="5"/>
+      <c r="R204" s="5"/>
+      <c r="S204" s="5"/>
+      <c r="T204" s="6"/>
+    </row>
+    <row r="205" spans="1:20">
+      <c r="B205" s="7"/>
+      <c r="C205" s="5"/>
+      <c r="D205" s="5"/>
+      <c r="E205" s="5"/>
+      <c r="F205" s="5"/>
+      <c r="G205" s="5"/>
+      <c r="H205" s="5"/>
+      <c r="I205" s="5"/>
+      <c r="J205" s="5"/>
+      <c r="K205" s="5"/>
+      <c r="L205" s="5"/>
+      <c r="M205" s="5"/>
+      <c r="N205" s="5"/>
+      <c r="O205" s="5"/>
+      <c r="P205" s="5"/>
+      <c r="Q205" s="5"/>
+      <c r="R205" s="5"/>
+      <c r="S205" s="5"/>
+      <c r="T205" s="6"/>
+    </row>
+    <row r="206" spans="1:20">
+      <c r="B206" s="7"/>
+      <c r="C206" s="5"/>
+      <c r="D206" s="5"/>
+      <c r="E206" s="5"/>
+      <c r="F206" s="5"/>
+      <c r="G206" s="5"/>
+      <c r="H206" s="5"/>
+      <c r="I206" s="5"/>
+      <c r="J206" s="5"/>
+      <c r="K206" s="5"/>
+      <c r="L206" s="5"/>
+      <c r="M206" s="5"/>
+      <c r="N206" s="5"/>
+      <c r="O206" s="5"/>
+      <c r="P206" s="5"/>
+      <c r="Q206" s="5"/>
+      <c r="R206" s="5"/>
+      <c r="S206" s="5"/>
+      <c r="T206" s="6"/>
+    </row>
+    <row r="207" spans="1:20">
+      <c r="B207" s="7"/>
+      <c r="C207" s="5"/>
+      <c r="D207" s="5"/>
+      <c r="E207" s="5"/>
+      <c r="F207" s="5"/>
+      <c r="G207" s="5"/>
+      <c r="H207" s="5"/>
+      <c r="I207" s="5"/>
+      <c r="J207" s="5"/>
+      <c r="K207" s="5"/>
+      <c r="L207" s="5"/>
+      <c r="M207" s="5"/>
+      <c r="N207" s="5"/>
+      <c r="O207" s="5"/>
+      <c r="P207" s="5"/>
+      <c r="Q207" s="5"/>
+      <c r="R207" s="5"/>
+      <c r="S207" s="5"/>
+      <c r="T207" s="6"/>
+    </row>
+    <row r="208" spans="1:20">
+      <c r="B208" s="7"/>
+      <c r="C208" s="5"/>
+      <c r="D208" s="5"/>
+      <c r="E208" s="5"/>
+      <c r="F208" s="5"/>
+      <c r="G208" s="5"/>
+      <c r="H208" s="5"/>
+      <c r="I208" s="5"/>
+      <c r="J208" s="5"/>
+      <c r="K208" s="5"/>
+      <c r="L208" s="5"/>
+      <c r="M208" s="5"/>
+      <c r="N208" s="5"/>
+      <c r="O208" s="5"/>
+      <c r="P208" s="5"/>
+      <c r="Q208" s="5"/>
+      <c r="R208" s="5"/>
+      <c r="S208" s="5"/>
+      <c r="T208" s="6"/>
+    </row>
+    <row r="209" spans="1:20">
+      <c r="B209" s="7"/>
+      <c r="C209" s="5"/>
+      <c r="D209" s="5"/>
+      <c r="E209" s="5"/>
+      <c r="F209" s="5"/>
+      <c r="G209" s="5"/>
+      <c r="H209" s="5"/>
+      <c r="I209" s="5"/>
+      <c r="J209" s="5"/>
+      <c r="K209" s="5"/>
+      <c r="L209" s="5"/>
+      <c r="M209" s="5"/>
+      <c r="N209" s="5"/>
+      <c r="O209" s="5"/>
+      <c r="P209" s="5"/>
+      <c r="Q209" s="5"/>
+      <c r="R209" s="5"/>
+      <c r="S209" s="5"/>
+      <c r="T209" s="6"/>
+    </row>
+    <row r="210" spans="1:20">
+      <c r="B210" s="7"/>
+      <c r="C210" s="5"/>
+      <c r="D210" s="5"/>
+      <c r="E210" s="5"/>
+      <c r="F210" s="5"/>
+      <c r="G210" s="5"/>
+      <c r="H210" s="5"/>
+      <c r="I210" s="5"/>
+      <c r="J210" s="5"/>
+      <c r="K210" s="5"/>
+      <c r="L210" s="5"/>
+      <c r="M210" s="5"/>
+      <c r="N210" s="5"/>
+      <c r="O210" s="5"/>
+      <c r="P210" s="5"/>
+      <c r="Q210" s="5"/>
+      <c r="R210" s="5"/>
+      <c r="S210" s="5"/>
+      <c r="T210" s="6"/>
+    </row>
+    <row r="211" spans="1:20">
+      <c r="B211" s="7"/>
+      <c r="C211" s="5"/>
+      <c r="D211" s="5"/>
+      <c r="E211" s="5"/>
+      <c r="F211" s="5"/>
+      <c r="G211" s="5"/>
+      <c r="H211" s="5"/>
+      <c r="I211" s="5"/>
+      <c r="J211" s="5"/>
+      <c r="K211" s="5"/>
+      <c r="L211" s="5"/>
+      <c r="M211" s="5"/>
+      <c r="N211" s="5"/>
+      <c r="O211" s="5"/>
+      <c r="P211" s="5"/>
+      <c r="Q211" s="5"/>
+      <c r="R211" s="5"/>
+      <c r="S211" s="5"/>
+      <c r="T211" s="6"/>
+    </row>
+    <row r="212" spans="1:20">
+      <c r="B212" s="7"/>
+      <c r="C212" s="5"/>
+      <c r="D212" s="5"/>
+      <c r="E212" s="5"/>
+      <c r="F212" s="5"/>
+      <c r="G212" s="5"/>
+      <c r="H212" s="5"/>
+      <c r="I212" s="5"/>
+      <c r="J212" s="5"/>
+      <c r="K212" s="5"/>
+      <c r="L212" s="5"/>
+      <c r="M212" s="5"/>
+      <c r="N212" s="5"/>
+      <c r="O212" s="5"/>
+      <c r="P212" s="5"/>
+      <c r="Q212" s="5"/>
+      <c r="R212" s="5"/>
+      <c r="S212" s="5"/>
+      <c r="T212" s="6"/>
+    </row>
+    <row r="213" spans="1:20">
+      <c r="B213" s="7"/>
+      <c r="C213" s="5"/>
+      <c r="D213" s="5"/>
+      <c r="E213" s="5"/>
+      <c r="F213" s="5"/>
+      <c r="G213" s="5"/>
+      <c r="H213" s="5"/>
+      <c r="I213" s="5"/>
+      <c r="J213" s="5"/>
+      <c r="K213" s="5"/>
+      <c r="L213" s="5"/>
+      <c r="M213" s="5"/>
+      <c r="N213" s="5"/>
+      <c r="O213" s="5"/>
+      <c r="P213" s="5"/>
+      <c r="Q213" s="5"/>
+      <c r="R213" s="5"/>
+      <c r="S213" s="5"/>
+      <c r="T213" s="6"/>
+    </row>
+    <row r="214" spans="1:20">
+      <c r="B214" s="8"/>
+      <c r="C214" s="9"/>
+      <c r="D214" s="9"/>
+      <c r="E214" s="9"/>
+      <c r="F214" s="9"/>
+      <c r="G214" s="9"/>
+      <c r="H214" s="9"/>
+      <c r="I214" s="9"/>
+      <c r="J214" s="9"/>
+      <c r="K214" s="9"/>
+      <c r="L214" s="9"/>
+      <c r="M214" s="9"/>
+      <c r="N214" s="9"/>
+      <c r="O214" s="9"/>
+      <c r="P214" s="9"/>
+      <c r="Q214" s="9"/>
+      <c r="R214" s="9"/>
+      <c r="S214" s="9"/>
+      <c r="T214" s="10"/>
+    </row>
+    <row r="217" spans="1:20">
+      <c r="A217" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="B217" s="2"/>
+      <c r="C217" s="2"/>
+      <c r="D217" s="2"/>
+      <c r="E217" s="2"/>
+      <c r="F217" s="2"/>
+      <c r="G217" s="2"/>
+      <c r="H217" s="2"/>
+      <c r="I217" s="2"/>
+      <c r="J217" s="2"/>
+      <c r="K217" s="2"/>
+      <c r="L217" s="2"/>
+      <c r="M217" s="2"/>
+      <c r="N217" s="2"/>
+      <c r="O217" s="2"/>
+      <c r="P217" s="2"/>
+      <c r="Q217" s="3"/>
+    </row>
+    <row r="218" spans="1:20">
+      <c r="A218" s="7"/>
+      <c r="B218" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="C218" s="5"/>
+      <c r="D218" s="5"/>
+      <c r="E218" s="5"/>
+      <c r="F218" s="5"/>
+      <c r="G218" s="5"/>
+      <c r="H218" s="5"/>
+      <c r="I218" s="5"/>
+      <c r="J218" s="5"/>
+      <c r="K218" s="5"/>
+      <c r="L218" s="5"/>
+      <c r="M218" s="5"/>
+      <c r="N218" s="5"/>
+      <c r="O218" s="5"/>
+      <c r="P218" s="5"/>
+      <c r="Q218" s="6"/>
+    </row>
+    <row r="219" spans="1:20">
+      <c r="A219" s="7"/>
+      <c r="B219" s="5"/>
+      <c r="C219" s="5"/>
+      <c r="D219" s="5"/>
+      <c r="E219" s="5"/>
+      <c r="F219" s="5"/>
+      <c r="G219" s="5"/>
+      <c r="H219" s="5"/>
+      <c r="I219" s="5"/>
+      <c r="J219" s="5"/>
+      <c r="K219" s="5"/>
+      <c r="L219" s="5"/>
+      <c r="M219" s="5"/>
+      <c r="N219" s="5"/>
+      <c r="O219" s="5"/>
+      <c r="P219" s="5"/>
+      <c r="Q219" s="6"/>
+    </row>
+    <row r="220" spans="1:20">
+      <c r="A220" s="7"/>
+      <c r="B220" s="5"/>
+      <c r="C220" s="5"/>
+      <c r="D220" s="5"/>
+      <c r="E220" s="5"/>
+      <c r="F220" s="5"/>
+      <c r="G220" s="5"/>
+      <c r="H220" s="5"/>
+      <c r="I220" s="5"/>
+      <c r="J220" s="5"/>
+      <c r="K220" s="5"/>
+      <c r="L220" s="5"/>
+      <c r="M220" s="5"/>
+      <c r="N220" s="5"/>
+      <c r="O220" s="5"/>
+      <c r="P220" s="5"/>
+      <c r="Q220" s="6"/>
+    </row>
+    <row r="221" spans="1:20">
+      <c r="A221" s="7"/>
+      <c r="B221" s="5"/>
+      <c r="C221" s="5"/>
+      <c r="D221" s="5"/>
+      <c r="E221" s="5"/>
+      <c r="F221" s="5"/>
+      <c r="G221" s="5"/>
+      <c r="H221" s="5"/>
+      <c r="I221" s="5"/>
+      <c r="J221" s="5"/>
+      <c r="K221" s="5"/>
+      <c r="L221" s="5"/>
+      <c r="M221" s="5"/>
+      <c r="N221" s="5"/>
+      <c r="O221" s="5"/>
+      <c r="P221" s="5"/>
+      <c r="Q221" s="6"/>
+    </row>
+    <row r="222" spans="1:20">
+      <c r="A222" s="7"/>
+      <c r="B222" s="5"/>
+      <c r="C222" s="5"/>
+      <c r="D222" s="5"/>
+      <c r="E222" s="5"/>
+      <c r="F222" s="5"/>
+      <c r="G222" s="5"/>
+      <c r="H222" s="5"/>
+      <c r="I222" s="5"/>
+      <c r="J222" s="5"/>
+      <c r="K222" s="5"/>
+      <c r="L222" s="5"/>
+      <c r="M222" s="5"/>
+      <c r="N222" s="5"/>
+      <c r="O222" s="5"/>
+      <c r="P222" s="5"/>
+      <c r="Q222" s="6"/>
+    </row>
+    <row r="223" spans="1:20">
+      <c r="A223" s="7"/>
+      <c r="B223" s="5"/>
+      <c r="C223" s="5"/>
+      <c r="D223" s="5"/>
+      <c r="E223" s="5"/>
+      <c r="F223" s="5"/>
+      <c r="G223" s="5"/>
+      <c r="H223" s="5"/>
+      <c r="I223" s="5"/>
+      <c r="J223" s="5"/>
+      <c r="K223" s="5"/>
+      <c r="L223" s="5"/>
+      <c r="M223" s="5"/>
+      <c r="N223" s="5"/>
+      <c r="O223" s="5"/>
+      <c r="P223" s="5"/>
+      <c r="Q223" s="6"/>
+    </row>
+    <row r="224" spans="1:20">
+      <c r="A224" s="7"/>
+      <c r="B224" s="5"/>
+      <c r="C224" s="5"/>
+      <c r="D224" s="5"/>
+      <c r="E224" s="5"/>
+      <c r="F224" s="5"/>
+      <c r="G224" s="5"/>
+      <c r="H224" s="5"/>
+      <c r="I224" s="5"/>
+      <c r="J224" s="5"/>
+      <c r="K224" s="5"/>
+      <c r="L224" s="5"/>
+      <c r="M224" s="5"/>
+      <c r="N224" s="5"/>
+      <c r="O224" s="5"/>
+      <c r="P224" s="5"/>
+      <c r="Q224" s="6"/>
+    </row>
+    <row r="225" spans="1:17">
+      <c r="A225" s="7"/>
+      <c r="B225" s="5"/>
+      <c r="C225" s="5"/>
+      <c r="D225" s="5"/>
+      <c r="E225" s="5"/>
+      <c r="F225" s="5"/>
+      <c r="G225" s="5"/>
+      <c r="H225" s="5"/>
+      <c r="I225" s="5"/>
+      <c r="J225" s="5"/>
+      <c r="K225" s="5"/>
+      <c r="L225" s="5"/>
+      <c r="M225" s="5"/>
+      <c r="N225" s="5"/>
+      <c r="O225" s="5"/>
+      <c r="P225" s="5"/>
+      <c r="Q225" s="6"/>
+    </row>
+    <row r="226" spans="1:17">
+      <c r="A226" s="7"/>
+      <c r="B226" s="5"/>
+      <c r="C226" s="5"/>
+      <c r="D226" s="5"/>
+      <c r="E226" s="5"/>
+      <c r="F226" s="5"/>
+      <c r="G226" s="5"/>
+      <c r="H226" s="5"/>
+      <c r="I226" s="5"/>
+      <c r="J226" s="5"/>
+      <c r="K226" s="5"/>
+      <c r="L226" s="5"/>
+      <c r="M226" s="5"/>
+      <c r="N226" s="5"/>
+      <c r="O226" s="5"/>
+      <c r="P226" s="5"/>
+      <c r="Q226" s="6"/>
+    </row>
+    <row r="227" spans="1:17">
+      <c r="A227" s="7"/>
+      <c r="B227" s="5"/>
+      <c r="C227" s="5"/>
+      <c r="D227" s="5"/>
+      <c r="E227" s="5"/>
+      <c r="F227" s="5"/>
+      <c r="G227" s="5"/>
+      <c r="H227" s="5"/>
+      <c r="I227" s="5"/>
+      <c r="J227" s="5"/>
+      <c r="K227" s="5"/>
+      <c r="L227" s="5"/>
+      <c r="M227" s="5"/>
+      <c r="N227" s="5"/>
+      <c r="O227" s="5"/>
+      <c r="P227" s="5"/>
+      <c r="Q227" s="6"/>
+    </row>
+    <row r="228" spans="1:17">
+      <c r="A228" s="7"/>
+      <c r="B228" s="5"/>
+      <c r="C228" s="5"/>
+      <c r="D228" s="5"/>
+      <c r="E228" s="5"/>
+      <c r="F228" s="5"/>
+      <c r="G228" s="5"/>
+      <c r="H228" s="5"/>
+      <c r="I228" s="5"/>
+      <c r="J228" s="5"/>
+      <c r="K228" s="5"/>
+      <c r="L228" s="5"/>
+      <c r="M228" s="5"/>
+      <c r="N228" s="5"/>
+      <c r="O228" s="5"/>
+      <c r="P228" s="5"/>
+      <c r="Q228" s="6"/>
+    </row>
+    <row r="229" spans="1:17">
+      <c r="A229" s="7"/>
+      <c r="B229" s="5"/>
+      <c r="C229" s="5"/>
+      <c r="D229" s="5"/>
+      <c r="E229" s="5"/>
+      <c r="F229" s="5"/>
+      <c r="G229" s="5"/>
+      <c r="H229" s="5"/>
+      <c r="I229" s="5"/>
+      <c r="J229" s="5"/>
+      <c r="K229" s="5"/>
+      <c r="L229" s="5"/>
+      <c r="M229" s="5"/>
+      <c r="N229" s="5"/>
+      <c r="O229" s="5"/>
+      <c r="P229" s="5"/>
+      <c r="Q229" s="6"/>
+    </row>
+    <row r="230" spans="1:17">
+      <c r="A230" s="7"/>
+      <c r="B230" s="5"/>
+      <c r="C230" s="5"/>
+      <c r="D230" s="5"/>
+      <c r="E230" s="5"/>
+      <c r="F230" s="5"/>
+      <c r="G230" s="5"/>
+      <c r="H230" s="5"/>
+      <c r="I230" s="5"/>
+      <c r="J230" s="5"/>
+      <c r="K230" s="5"/>
+      <c r="L230" s="5"/>
+      <c r="M230" s="5"/>
+      <c r="N230" s="5"/>
+      <c r="O230" s="5"/>
+      <c r="P230" s="5"/>
+      <c r="Q230" s="6"/>
+    </row>
+    <row r="231" spans="1:17">
+      <c r="A231" s="7"/>
+      <c r="B231" s="5"/>
+      <c r="C231" s="5"/>
+      <c r="D231" s="5"/>
+      <c r="E231" s="5"/>
+      <c r="F231" s="5"/>
+      <c r="G231" s="5"/>
+      <c r="H231" s="5"/>
+      <c r="I231" s="5"/>
+      <c r="J231" s="5"/>
+      <c r="K231" s="5"/>
+      <c r="L231" s="5"/>
+      <c r="M231" s="5"/>
+      <c r="N231" s="5"/>
+      <c r="O231" s="5"/>
+      <c r="P231" s="5"/>
+      <c r="Q231" s="6"/>
+    </row>
+    <row r="232" spans="1:17">
+      <c r="A232" s="7"/>
+      <c r="B232" s="5"/>
+      <c r="C232" s="5"/>
+      <c r="D232" s="5"/>
+      <c r="E232" s="5"/>
+      <c r="F232" s="5"/>
+      <c r="G232" s="5"/>
+      <c r="H232" s="5"/>
+      <c r="I232" s="5"/>
+      <c r="J232" s="5"/>
+      <c r="K232" s="5"/>
+      <c r="L232" s="5"/>
+      <c r="M232" s="5"/>
+      <c r="N232" s="5"/>
+      <c r="O232" s="5"/>
+      <c r="P232" s="5"/>
+      <c r="Q232" s="6"/>
+    </row>
+    <row r="233" spans="1:17">
+      <c r="A233" s="7"/>
+      <c r="B233" s="5"/>
+      <c r="C233" s="5"/>
+      <c r="D233" s="5"/>
+      <c r="E233" s="5"/>
+      <c r="F233" s="5"/>
+      <c r="G233" s="5"/>
+      <c r="H233" s="5"/>
+      <c r="I233" s="5"/>
+      <c r="J233" s="5"/>
+      <c r="K233" s="5"/>
+      <c r="L233" s="5"/>
+      <c r="M233" s="5"/>
+      <c r="N233" s="5"/>
+      <c r="O233" s="5"/>
+      <c r="P233" s="5"/>
+      <c r="Q233" s="6"/>
+    </row>
+    <row r="234" spans="1:17">
+      <c r="A234" s="7"/>
+      <c r="B234" s="5"/>
+      <c r="C234" s="5"/>
+      <c r="D234" s="5"/>
+      <c r="E234" s="5"/>
+      <c r="F234" s="5"/>
+      <c r="G234" s="5"/>
+      <c r="H234" s="5"/>
+      <c r="I234" s="5"/>
+      <c r="J234" s="5"/>
+      <c r="K234" s="5"/>
+      <c r="L234" s="5"/>
+      <c r="M234" s="5"/>
+      <c r="N234" s="5"/>
+      <c r="O234" s="5"/>
+      <c r="P234" s="5"/>
+      <c r="Q234" s="6"/>
+    </row>
+    <row r="235" spans="1:17">
+      <c r="A235" s="7"/>
+      <c r="B235" s="5"/>
+      <c r="C235" s="5"/>
+      <c r="D235" s="5"/>
+      <c r="E235" s="5"/>
+      <c r="F235" s="5"/>
+      <c r="G235" s="5"/>
+      <c r="H235" s="5"/>
+      <c r="I235" s="5"/>
+      <c r="J235" s="5"/>
+      <c r="K235" s="5"/>
+      <c r="L235" s="5"/>
+      <c r="M235" s="5"/>
+      <c r="N235" s="5"/>
+      <c r="O235" s="5"/>
+      <c r="P235" s="5"/>
+      <c r="Q235" s="6"/>
+    </row>
+    <row r="236" spans="1:17">
+      <c r="A236" s="7"/>
+      <c r="B236" s="5"/>
+      <c r="C236" s="5"/>
+      <c r="D236" s="5"/>
+      <c r="E236" s="5"/>
+      <c r="F236" s="5"/>
+      <c r="G236" s="5"/>
+      <c r="H236" s="5"/>
+      <c r="I236" s="5"/>
+      <c r="J236" s="5"/>
+      <c r="K236" s="5"/>
+      <c r="L236" s="5"/>
+      <c r="M236" s="5"/>
+      <c r="N236" s="5"/>
+      <c r="O236" s="5"/>
+      <c r="P236" s="5"/>
+      <c r="Q236" s="6"/>
+    </row>
+    <row r="237" spans="1:17">
+      <c r="A237" s="8"/>
+      <c r="B237" s="9"/>
+      <c r="C237" s="9"/>
+      <c r="D237" s="9"/>
+      <c r="E237" s="9"/>
+      <c r="F237" s="9"/>
+      <c r="G237" s="9"/>
+      <c r="H237" s="9"/>
+      <c r="I237" s="9"/>
+      <c r="J237" s="9"/>
+      <c r="K237" s="9"/>
+      <c r="L237" s="9"/>
+      <c r="M237" s="9"/>
+      <c r="N237" s="9"/>
+      <c r="O237" s="9"/>
+      <c r="P237" s="9"/>
+      <c r="Q237" s="10"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>